<commit_message>
severe changes applied to production as per client request
</commit_message>
<xml_diff>
--- a/app/build/exe.win-amd64-3.13/database/question_bank.xlsx
+++ b/app/build/exe.win-amd64-3.13/database/question_bank.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G70"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,19 +471,17 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>7XAEW4</t>
-        </is>
+      <c r="A2" t="n">
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>What happens when dilute hydrochloric acid is added to iron filling ?</t>
+          <t>Choose the correctly spelled word:</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>English</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -491,7 +489,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Hydrogen gas and iron chloride are produced, Chlorine gas and iron hydroxide are produced, No reaction takes place, Iron salt and water are produced</t>
+          <t>ascept, Accept, accepe, eccept</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -501,24 +499,22 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Hydrogen gas and iron chloride are produced</t>
+          <t>Accept</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>GAIJQ5</t>
-        </is>
+      <c r="A3" t="n">
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>The solution of FeO + Chlorine  turns ___________ due to formation of iron (II) chloride (FeCl2).</t>
+          <t>How do you correctly spell the word: 'accidentally'?</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>English</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -526,7 +522,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Brown, Yellow, Light Blue, Light green</t>
+          <t>Accidentally, eccidentally, ascidentally, accidentalle</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -536,24 +532,22 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Light green</t>
+          <t>Accidentally</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>G53HIP</t>
-        </is>
+      <c r="A4" t="n">
+        <v>3</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>A student added dilute HCL to a test tube containing zinc granules and made following observations:</t>
+          <t>How do you correctly spell the word: 'accommodate'?</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>English</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -561,7 +555,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>The zinc surface become dull and black, A gas evolved which burnt with a pop sound., The solution remains colourless, The solution becomes green in colour.</t>
+          <t>ascommodate, eccommodate, accommodate, Accommodate</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -571,24 +565,22 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>A gas evolved which burnt with a pop sound.</t>
+          <t>accommodate</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>T9VG59</t>
-        </is>
+      <c r="A5" t="n">
+        <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Which of the following reactions will produce effervescence due to gas formation ?</t>
+          <t>Choose the correctly spelled word:</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>English</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -596,7 +588,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Copper (Cu) reacting with dilute hydrochloric acid (HCL), Zinc (Zn) reacting with dilute sulfuric acid (H2SO4), Iron (Fe) reacting with copper sulphate (CuSO4) solution, Sodium chloride (Nacl) disolving in water</t>
+          <t>echieve, Achieve, ashieve, achieve</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -606,24 +598,22 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Zinc (Zn) reacting with dilute sulfuric acid (H2SO4)</t>
+          <t>Achieve</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>COQGWW</t>
-        </is>
+      <c r="A6" t="n">
+        <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Which of the following reactions will produce effervescence due to carbon dioxide gas (CO2) ?</t>
+          <t>Choose the correctly spelled word:</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>English</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -631,7 +621,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Mg reacting with HCL, Na2Co3 reacting with H2SO4, Iron (Fe) reacting with hydrochloric acid (HCL), Copper (Cu) reacting with dilute nitric acid (HNO3)</t>
+          <t>Acquire, asquire, acquire, ecquire</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -641,24 +631,22 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Na2Co3 reacting with H2SO4</t>
+          <t>Acquire</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>70FLE9</t>
-        </is>
+      <c r="A7" t="n">
+        <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>The reaction of Hydrogen (H2) gas with Oxygen gas to form water is an example of</t>
+          <t>Choose the correctly spelled word:</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>English</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -666,7 +654,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Combination reaction, Redox reaction, Exothermic reaction, All of these reaction</t>
+          <t>address, addrese, Address, eddress</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -676,24 +664,22 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>All of these reaction</t>
+          <t>address</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>50N9GH</t>
-        </is>
+      <c r="A8" t="n">
+        <v>7</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>The blue flame in the below image represents the burning of which metal ?</t>
+          <t>How do you correctly spell the word: 'adequate'?</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>English</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -701,7 +687,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Iron, Copper, Sodium, All metal burn to give a blue flame</t>
+          <t>adequate, edequate, Adequate, adequate</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -711,24 +697,22 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Copper</t>
+          <t>adequate</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>X3WOWW</t>
-        </is>
+      <c r="A9" t="n">
+        <v>8</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>The yellow flame is observed on burning which metal ?</t>
+          <t>Choose the correctly spelled word:</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>English</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -736,7 +720,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Copper, Iron, Potassium, Sodium</t>
+          <t>adjourn, edjourn, adjoure, Adjourn</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -746,24 +730,22 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Sodium</t>
+          <t>adjourn</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>QTBND8</t>
-        </is>
+      <c r="A10" t="n">
+        <v>9</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>The purple flame is observed on burning which metal ?</t>
+          <t>Choose the correctly spelled word:</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>English</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -771,7 +753,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Potassium, Calcium, Barium, Strontium</t>
+          <t>edvantageous, Advantageous, advantageous, advantageoue</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -781,24 +763,22 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Potassium</t>
+          <t>Advantageous</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>N1J43L</t>
-        </is>
+      <c r="A11" t="n">
+        <v>10</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>In the context of redox reaction the removal of hydrogen from a substance is known as ____.</t>
+          <t>Choose the correctly spelled word:</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>English</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -806,7 +786,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Oxidation, Dehydration, Dehydrogenation, Reduction</t>
+          <t>advertisement, edvertisement, advertisemene, Advertisement</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -816,24 +796,22 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Oxidation</t>
+          <t>advertisement</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>LT82ME</t>
-        </is>
+      <c r="A12" t="n">
+        <v>11</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>In the context of redox reaction the removal of oxygen from a substance is known as ____.</t>
+          <t>Choose the correctly spelled word:</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>English</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -841,7 +819,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Reduction, Dehydration, Dehydrogenation, Oxidation</t>
+          <t>advise, Advice, edvice, advice</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -851,24 +829,22 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Reduction</t>
+          <t>Advice</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>78YVOX</t>
-        </is>
+      <c r="A13" t="n">
+        <v>12</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Dissolving sugar is an example of</t>
+          <t>Choose the correctly spelled word:</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>English</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -876,7 +852,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Physical Change, Chemical Change, Redox Reaction, None of these</t>
+          <t>affest, affece, Affect, effect</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -886,24 +862,22 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Physical Change</t>
+          <t>Affect</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>G1LQHU</t>
-        </is>
+      <c r="A14" t="n">
+        <v>13</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>CuSO4 + Zn -&gt; Cu + ZnSO4 reaction is an example of a:</t>
+          <t>How do you correctly spell the word: 'aggravate'?</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>English</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -911,7 +885,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Double displacement reaction, Displacement reaction, Combination reaction, Decomposition reaction</t>
+          <t>aggravate, eggravate, aggravate, Aggravate</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -921,24 +895,22 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Displacement reaction</t>
+          <t>aggravate</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>VADHNJ</t>
-        </is>
+      <c r="A15" t="n">
+        <v>14</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>What happens when dilute hydrochloric acid is added to Zn Granuels ?</t>
+          <t>How do you correctly spell the word: 'all right'?</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>English</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -946,7 +918,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Zinc salt and water are produced, No reactions takes place, Hyrdogen gas and Zinc chloride are produced, Chlorine gas and Zinc hydroxide are produced</t>
+          <t>Al right, All right, Alright, Allright</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -956,25 +928,22 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Hyrdogen gas and Zinc chloride are produced</t>
+          <t>All right</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>BZFK8L</t>
-        </is>
+      <c r="A16" t="n">
+        <v>15</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Translate the following statements into chemical equation and then balance it. 
-Barium chloride reacts with aluminium sulphate to give aluminium sulphate to give aluminium chloride and a precipitate of barium sulphate.</t>
+          <t>Choose the correctly spelled word:</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>English</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -982,7 +951,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>BaCl₂ + Al₂(SO₄)₃ → AlCl₃ + BaSO₄, 3BaCl₂ + Al₂(SO₄)₃ → 2AlCl₃ + 3BaSO₄, 3BaCl₂ + 2Al₂(SO₄)₃ → 3AlCl₃ + 4BaSO₄, None of above</t>
+          <t>allot, alloe, ellot, Allot</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -992,26 +961,22 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>3BaCl₂ + Al₂(SO₄)₃ → 2AlCl₃ + 3BaSO₄</t>
+          <t>allot</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>4AY3AY</t>
-        </is>
+      <c r="A17" t="n">
+        <v>16</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Identify the type of reaction in each case
-a. Zinc Carbonate (s) 	​→ Zinc Oxide (s) + Carbon dioxide (g)
-b. Hydrogen (g) + Chlorine (g) → Hydrogen Chloride (g)</t>
+          <t>How do you correctly spell the word: 'amateur'?</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>English</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -1019,7 +984,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Thermal Decompostion , Combination reaction, Decomposition, Redox Reaction + Combination reaction, Displacement , Combination reaction, None of Above</t>
+          <t>emateur, amateur, amateue, Amateur</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1029,24 +994,22 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Decomposition, Redox Reaction + Combination reaction</t>
+          <t>amateur</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>OGD84M</t>
-        </is>
+      <c r="A18" t="n">
+        <v>17</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>The balancing equations is in accordance with of chemical :</t>
+          <t>Choose the correctly spelled word:</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>English</t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -1054,7 +1017,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Law of Combining Volumes, Law of Constant Proportions, Law of Conservation of mass, Both B and C</t>
+          <t>analysie, Analysis, enalysis, analysis</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1064,24 +1027,22 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Law of Conservation of mass</t>
+          <t>Analysis</t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>LA7C5Q</t>
-        </is>
+      <c r="A19" t="n">
+        <v>18</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>What type of reaction is respiration</t>
+          <t>Choose the correctly spelled word:</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>English</t>
         </is>
       </c>
       <c r="D19" t="n">
@@ -1089,7 +1050,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Exothermic reaction, Endothermic reaction, Reduction reaction, Combination reaction</t>
+          <t>enalyze, analyze, analyze, Analyze</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1099,32 +1060,26 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Exothermic reaction</t>
+          <t>analyze</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>75PAK1</t>
-        </is>
+      <c r="A20" t="n">
+        <v>19</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>A solution of a substance 'X' is used for white washing. Name the substance 'X' and write its chemical formula.</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Chemistry</t>
-        </is>
-      </c>
+          <t>Choose the correctly spelled word:</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr"/>
       <c r="D20" t="n">
         <v>2</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Lime Stone, CaCO3, Lime, CaCO3, Calcium Oxide, CaO, Calcium Carbonate, CaCO3</t>
+          <t>Relevent, Relevant, Relivant, Relavant</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1134,24 +1089,22 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Calcium Oxide, CaO</t>
+          <t>Relevant</t>
         </is>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>A24NZ0</t>
-        </is>
+      <c r="A21" t="n">
+        <v>20</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Write the balanced reaction of Calcium Oxide with water and state what type of reaction is this.</t>
+          <t>Choose the correctly spelled word:</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>English</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -1159,7 +1112,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>CaO + H2O → CaOH + H2, displacement, CaO + H2O → Ca(OH), combination reaction, CaO + H2O → Ca(OH)2, decomposition reaction, CaO + H2O → CaOH, Combination reaction</t>
+          <t>epparent, apparent, apparene, Apparent</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1169,24 +1122,22 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>CaO + H2O → Ca(OH), combination reaction</t>
+          <t>apparent</t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>AR9ODU</t>
-        </is>
+      <c r="A22" t="n">
+        <v>21</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>The reaction in which two compounds exchange their ions to form two new compounds is -</t>
+          <t>Choose the correctly spelled word:</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>English</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -1194,7 +1145,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>a displacement reaction, a decomposition reaction, an isomerization reaction, a double displacement reaction</t>
+          <t>ergument, Argument, argumene, argument</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1204,24 +1155,22 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>a double displacement reaction</t>
+          <t>Argument</t>
         </is>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>FAJHV9</t>
-        </is>
+      <c r="A23" t="n">
+        <v>22</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>When green coloured ferrous sulphate crystals are heated, the colour of the crystal changes because</t>
+          <t>Choose the correctly spelled word:</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>English</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -1229,7 +1178,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>It is decomposed to ferric oxide, It loses water of crystallisation, It forms SO3, it forms SO2</t>
+          <t>essociate, Associate, assosiate, associate</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1239,24 +1188,22 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>It loses water of crystallisation</t>
+          <t>Associate</t>
         </is>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>TQ7XRI</t>
-        </is>
+      <c r="A24" t="n">
+        <v>23</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>A compound used for white washing is</t>
+          <t>Choose the correctly spelled word:</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>English</t>
         </is>
       </c>
       <c r="D24" t="n">
@@ -1264,7 +1211,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Quick lime, Slaked Lime, Blue Vitriol, Limestone</t>
+          <t>atmosphere, Atmosphere, etmosphere, atmosphere</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -1274,24 +1221,22 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Quick lime</t>
+          <t>atmosphere</t>
         </is>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>EF2SVI</t>
-        </is>
+      <c r="A25" t="n">
+        <v>24</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Color of Magnesium oxide is</t>
+          <t>How do you correctly spell the word: 'available'?</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>English</t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -1299,7 +1244,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>White, Blue, Grey, Pink</t>
+          <t>available, available, evailable, Available</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -1309,24 +1254,22 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>White</t>
+          <t>available</t>
         </is>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>QKCYU3</t>
-        </is>
+      <c r="A26" t="n">
+        <v>25</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>A substance x is an oxide of an group 2 element is used in cement industry. On treatment with water it forms solution which turns red litmus to blue. Identify X ?</t>
+          <t>Choose the correctly spelled word:</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>English</t>
         </is>
       </c>
       <c r="D26" t="n">
@@ -1334,7 +1277,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Slaked Lime, Quick lime, Silver Sulphide, Limestone</t>
+          <t>ewkward, Awkward, awkware, awkward</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1344,24 +1287,22 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Quick lime</t>
+          <t>Awkward</t>
         </is>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>0NN9V5</t>
-        </is>
+      <c r="A27" t="n">
+        <v>26</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Which of the following is true for an unbalanced chemical equation ?</t>
+          <t>Choose the correctly spelled word:</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>English</t>
         </is>
       </c>
       <c r="D27" t="n">
@@ -1369,7 +1310,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Number of atom is equal on both sides of the equation, Number of atoms is less on the left side of the equation, Number of atoms is more on the right side of the equation, Both B and C</t>
+          <t>backware, Backward, beckward, baskward</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -1379,24 +1320,22 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Both B and C</t>
+          <t>Backward</t>
         </is>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>53BDJM</t>
-        </is>
+      <c r="A28" t="n">
+        <v>27</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Which reactant is reduced in given reaction CuO + H2 → Cu + H2O</t>
+          <t>Choose the correctly spelled word:</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>English</t>
         </is>
       </c>
       <c r="D28" t="n">
@@ -1404,7 +1343,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Copper Oxide, Oxygen, Hydrogen, None of Above</t>
+          <t>competitive, sompetitive, Competitive, competitive</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -1414,24 +1353,22 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Copper Oxide</t>
+          <t>competitive</t>
         </is>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>8SJKS8</t>
-        </is>
+      <c r="A29" t="n">
+        <v>28</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Which of the following does not involve a chemical reaction ?</t>
+          <t>Choose the correctly spelled word:</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>English</t>
         </is>
       </c>
       <c r="D29" t="n">
@@ -1439,7 +1376,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Digestion of food in our body, Process of Respiration, Burning of candle wax when heated, Melting of candle wax on heating</t>
+          <t>conscience, Conscience, conscience, sonscience</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -1449,24 +1386,22 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Melting of candle wax on heating</t>
+          <t>conscience</t>
         </is>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>6XPM6U</t>
-        </is>
+      <c r="A30" t="n">
+        <v>29</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>The neutralization reaction between an acid and a base is a type of</t>
+          <t>How do you correctly spell the word: 'conscientious'?</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>English</t>
         </is>
       </c>
       <c r="D30" t="n">
@@ -1474,7 +1409,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>double displacement reaction, displacement reaction, addition reaction, Decomposition reaction</t>
+          <t>Conscientious, conscientioue, sonscientious, conscientious</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -1484,24 +1419,22 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>double displacement reaction</t>
+          <t>Conscientious</t>
         </is>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>LST589</t>
-        </is>
+      <c r="A31" t="n">
+        <v>30</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>The neutralization reaction between an acid and base is a type of</t>
+          <t>Choose the correctly spelled word:</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>English</t>
         </is>
       </c>
       <c r="D31" t="n">
@@ -1509,7 +1442,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Endothermic, Exothermic, Amphoteric, None of Above</t>
+          <t>consensue, sonsensus, consensus, Consensus</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -1519,29 +1452,22 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Exothermic</t>
+          <t>consensus</t>
         </is>
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>EPPKOH</t>
-        </is>
+      <c r="A32" t="n">
+        <v>31</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Which of the following statement about the reaction below are incorrect ?
-2PbO(s) C(s) → 2 Pb(s) CO2 (g)
-1. lead is getting reduced
-2. Carbon dioxide is getting oxidised
-3. Carbon is getting oxidised
-4. Carbon is getting oxidised</t>
+          <t>Choose the correctly spelled word:</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>English</t>
         </is>
       </c>
       <c r="D32" t="n">
@@ -1549,7 +1475,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>1 and 2, 1 and 3, 1, 2 and 3, all of above</t>
+          <t>sonvenience, Convenience, convenience, convenience</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -1559,24 +1485,22 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>1 and 2</t>
+          <t>Convenience</t>
         </is>
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>N1OW20</t>
-        </is>
+      <c r="A33" t="n">
+        <v>32</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>On immersing an iron nail in CuSO4 solution for a few minutes, you will observe</t>
+          <t>Choose the correctly spelled word:</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>English</t>
         </is>
       </c>
       <c r="D33" t="n">
@@ -1584,7 +1508,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>No reaction takes place, The color of solution fades away, The Surface of iron nails acquire a balck coating, The color of solution changes to green</t>
+          <t>Critiscise, Critiscize, Criticise, Criticize</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -1594,24 +1518,22 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>The color of solution fades away</t>
+          <t>Criticize</t>
         </is>
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>BPCYDQ</t>
-        </is>
+      <c r="A34" t="n">
+        <v>33</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Which of the following is not physical change ?</t>
+          <t>Choose the correctly spelled word:</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>English</t>
         </is>
       </c>
       <c r="D34" t="n">
@@ -1619,7 +1541,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Boiling of water to give water vapour, Melting of ice to give water, Dissolution of salt in water, Combustion of Liqedfied Petroleum Gas (LPG)</t>
+          <t>suriosity, Curiosity, curiosite, curiosity</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -1629,24 +1551,22 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Combustion of Liqedfied Petroleum Gas (LPG)</t>
+          <t>Curiosity</t>
         </is>
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>TIWV37</t>
-        </is>
+      <c r="A35" t="n">
+        <v>34</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>We store  silver chloride in a dark coloured bottle because it is</t>
+          <t>How do you correctly spell the word: 'definitely'?</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>English</t>
         </is>
       </c>
       <c r="D35" t="n">
@@ -1654,7 +1574,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>a white solid, undergoes redox reaction, to avoid action by sunlight, none of above</t>
+          <t>Definitely, definitely, definitele, definitely</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -1664,24 +1584,22 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>to avoid action by sunlight</t>
+          <t>Definitely</t>
         </is>
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>5BJ7ZF</t>
-        </is>
+      <c r="A36" t="n">
+        <v>35</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>In a chemical reaction between sulphuric acid and barium chloride solution the white precipitates formed are of :</t>
+          <t>Choose the correctly spelled word:</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>English</t>
         </is>
       </c>
       <c r="D36" t="n">
@@ -1689,7 +1607,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>HCL, BaSO4, SO4, CL</t>
+          <t>desperete, desperate, desperate, Desperate</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -1699,24 +1617,22 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>BaSO4</t>
+          <t>desperate</t>
         </is>
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>LNEQT0</t>
-        </is>
+      <c r="A37" t="n">
+        <v>36</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>A chemical reaction does not involve</t>
+          <t>Choose the correctly spelled word:</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>English</t>
         </is>
       </c>
       <c r="D37" t="n">
@@ -1724,7 +1640,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Formation of new substances entirely different properties than that of the reactants, Breaking of old chemical bonds and formations of new chemical bonds., Rearrangement of the atoms of reactants to form new products, Changing of atom of on element into those of another element to form new products.</t>
+          <t>diseppoint, disappoint, disappoine, Disappoint</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -1734,24 +1650,22 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Changing of atom of on element into those of another element to form new products.</t>
+          <t>disappoint</t>
         </is>
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>N8IB1Y</t>
-        </is>
+      <c r="A38" t="n">
+        <v>37</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>The displacement reaction between iron (III) oxide and a metal X is used for welding the rail tracks. Here X is :</t>
+          <t>Choose the correctly spelled word:</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>English</t>
         </is>
       </c>
       <c r="D38" t="n">
@@ -1759,7 +1673,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Copper granuels, Sodium pellets, Aluminium dust, Magnesium ribbon</t>
+          <t>dissetisfied, dissatisfied, Dissatisfied, dissatisfiee</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -1769,24 +1683,22 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Aluminium dust</t>
+          <t>dissatisfied</t>
         </is>
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>VSGQ08</t>
-        </is>
+      <c r="A39" t="n">
+        <v>38</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>When ferrous sulphate is heated strongly it undergoes decomposition to form ferric oxide as a main product accompanied by a change in color form</t>
+          <t>Choose the correctly spelled word:</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>English</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1794,7 +1706,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Blue to Green, Green to Brown, Green to Yellow, Brown to Green</t>
+          <t>emberrass, embarrase, Embarrass, embarrass</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -1804,24 +1716,22 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Green to Brown</t>
+          <t>Embarrass</t>
         </is>
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>PWYALW</t>
-        </is>
+      <c r="A40" t="n">
+        <v>39</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Before burning in air, the magnesium ribbon is cleaned by rubbing is cleaned rubbing with a sand paper to :</t>
+          <t>Choose the correctly spelled word:</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>English</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1829,7 +1739,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Make the ribbon surface shiner, Remove the layer of magnesium oxide from the ribbon surface, Remove the layer of magnesium carbonate from the ribbon surface, Remove the moisture from the ribbon surface</t>
+          <t>environment, environmene, environment, Environment</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -1839,24 +1749,22 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>Remove the layer of magnesium oxide from the ribbon surface</t>
+          <t>environment</t>
         </is>
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>69RHN0</t>
-        </is>
+      <c r="A41" t="n">
+        <v>40</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Oxidation is a process which involves</t>
+          <t>Choose the correctly spelled word:</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>English</t>
         </is>
       </c>
       <c r="D41" t="n">
@@ -1864,7 +1772,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>addition of oxygen, addition of hydrogen, removal of oxygen, removal of hydrogen</t>
+          <t>Exaggerate, exeggerate, exaggerate, exaggerate</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -1874,24 +1782,22 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>addition of oxygen</t>
+          <t>Exaggerate</t>
         </is>
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>2O4048</t>
-        </is>
+      <c r="A42" t="n">
+        <v>41</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Reduction is a process which involves</t>
+          <t>Choose the correctly spelled word:</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>English</t>
         </is>
       </c>
       <c r="D42" t="n">
@@ -1899,7 +1805,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>addition of hydrogen, removal of oxygen, removal of hydrogen, addition of oxygen</t>
+          <t>exsellent, excellene, excellent, Excellent</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -1909,24 +1815,22 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>removal of oxygen</t>
+          <t>excellent</t>
         </is>
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>HKPYMP</t>
-        </is>
+      <c r="A43" t="n">
+        <v>42</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>In an electrolytic cell where electrolysis is carried, anode has:</t>
+          <t>Choose the correctly spelled word:</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>English</t>
         </is>
       </c>
       <c r="D43" t="n">
@@ -1934,7 +1838,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Positive charge, Negative Charge, Connected to negative terminal of the better, None of these is correct</t>
+          <t>existence, Existence, existense, existence</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -1944,24 +1848,22 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>Positive charge</t>
+          <t>existence</t>
         </is>
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>HP2SKX</t>
-        </is>
+      <c r="A44" t="n">
+        <v>43</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>To indicate the presence of gaseous reactants or product, we use the symbol</t>
+          <t>Choose the correctly spelled word:</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>English</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -1969,7 +1871,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>(Product)g or (Reactant)g, (Product)- or (Reactant)-, (Product). or (reactant)., Both (a) and (b)</t>
+          <t>experience, experience, Experience, experiense</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -1979,24 +1881,22 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>(Product)g or (Reactant)g</t>
+          <t>experience</t>
         </is>
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>WHN56L</t>
-        </is>
+      <c r="A45" t="n">
+        <v>44</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Which of the following is a physical change ?</t>
+          <t>Choose the correctly spelled word:</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>English</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -2004,7 +1904,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Formation of curd from milk, Ripening of fruits, Getting salt from sea water, Burning of wood</t>
+          <t>familiar, femiliar, familiae, Familiar</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -2014,32 +1914,30 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Getting salt from sea water</t>
+          <t>familiar</t>
         </is>
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>5F2WOD</t>
-        </is>
+      <c r="A46" t="n">
+        <v>45</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Silver article turns black when kept in the open for a few days due to formation of</t>
+          <t>Choose the correctly spelled word:</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>English</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>H2S, AgS, AgSO4, Ag2S</t>
+          <t>Finally, finalle, finally, finelly</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -2049,24 +1947,22 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Ag2S</t>
+          <t>Finally</t>
         </is>
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>MOSNUK</t>
-        </is>
+      <c r="A47" t="n">
+        <v>46</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Which of the following is not a characteristic of a chemical reaction ?</t>
+          <t>Choose the correctly spelled word:</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>English</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -2074,7 +1970,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Change in state, Change in temperature, Evolution of gas, Evolution of liquid</t>
+          <t>fluorescene, fluorescent, Fluorescent, fluoressent</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -2084,24 +1980,22 @@
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Evolution of liquid</t>
+          <t>fluorescent</t>
         </is>
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>RQT32M</t>
-        </is>
+      <c r="A48" t="n">
+        <v>47</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Chemical formula of marble</t>
+          <t>Choose the correctly spelled word:</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>English</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -2109,7 +2003,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>CaO, Ca(OH)2, Mg(OH)2, CaCO3</t>
+          <t>foreseeeble, foreseeable, foreseeable, Foreseeable</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -2119,25 +2013,22 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>CaCO3</t>
+          <t>foreseeable</t>
         </is>
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>LAKUQ4</t>
-        </is>
+      <c r="A49" t="n">
+        <v>48</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>aMg3N2 + bH20 → cMg(OH)2 + dNH3
-when the equation is balanced, the coefficients a, b, c and d respectively are -</t>
+          <t>Choose the correctly spelled word:</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>English</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -2145,7 +2036,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>1, 6, 3, 2, 1, 3, 3, 2, 1, 2, 1, 3, 2, 3, 6, 2</t>
+          <t>fulfilline, Fulfilling, fulfilling, fulfilling</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -2155,24 +2046,22 @@
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>1, 6, 3, 2</t>
+          <t>Fulfilling</t>
         </is>
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>RT74J0</t>
-        </is>
+      <c r="A50" t="n">
+        <v>49</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>In the reaction xPb(NO3)2 → yPbO(s) + zNO2(g) + O2(g) Values of x, y and z respectively are</t>
+          <t>Choose the correctly spelled word:</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>English</t>
         </is>
       </c>
       <c r="D50" t="n">
@@ -2180,7 +2069,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>1, 1, 2, 2, 2, 4, 1, 2, 4, 4, 2, 2</t>
+          <t>Generally, generally, generelly, generalle</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -2190,24 +2079,22 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>2, 2, 4</t>
+          <t>Generally</t>
         </is>
       </c>
     </row>
     <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>FVKWNI</t>
-        </is>
+      <c r="A51" t="n">
+        <v>50</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>In the balanced equation Na2Co3 + xHCL → 2Nacl + CO2 + H2O. The value of x is ....</t>
+          <t>Choose the correctly spelled word:</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>English</t>
         </is>
       </c>
       <c r="D51" t="n">
@@ -2215,7 +2102,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>1, 2, 3, 4</t>
+          <t>government, Government, governmene, government</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -2225,673 +2112,7 @@
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>2</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>UMHHNQ</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>Lead nitrate Pb(NO3)2, on heating forms Lead oxide (PbO) solid and Nitrogen dioxide gas. What are the color of lead oxide and nitrogen dioxide ?</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>Chemistry</t>
-        </is>
-      </c>
-      <c r="D52" t="n">
-        <v>2</v>
-      </c>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>White, Colourless, White, Brown, Yellow, Brown, Yellow, Colourless</t>
-        </is>
-      </c>
-      <c r="F52" t="inlineStr">
-        <is>
-          <t>MCQ</t>
-        </is>
-      </c>
-      <c r="G52" t="inlineStr">
-        <is>
-          <t>Yellow, Brown</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>UB2ZFL</t>
-        </is>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>One of the following is an endothermic reaction. This is</t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>Chemistry</t>
-        </is>
-      </c>
-      <c r="D53" t="n">
-        <v>2</v>
-      </c>
-      <c r="E53" t="inlineStr">
-        <is>
-          <t>Combination of carbon and oxygen to form carbon monoxide, Combination of nitrogen and oxygen to form nitrogen monoxide, Combination of glucose and oxygen to form carbon dioxide and water, Combination of zinc and hcl form zinc chloride and hydrogen</t>
-        </is>
-      </c>
-      <c r="F53" t="inlineStr">
-        <is>
-          <t>MCQ</t>
-        </is>
-      </c>
-      <c r="G53" t="inlineStr">
-        <is>
-          <t>Combination of nitrogen and oxygen to form nitrogen monoxide</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>FIPHHO</t>
-        </is>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>Name of the products formed when iron fillings are heated with dillute hydrochloric acid</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>Chemistry</t>
-        </is>
-      </c>
-      <c r="D54" t="n">
-        <v>2</v>
-      </c>
-      <c r="E54" t="inlineStr">
-        <is>
-          <t>Fe (III) chloride and water, Fe (II) chloride and water, Fe (II) chloride and hydrogen gas, Fe (III) chloride and hydrogen gas</t>
-        </is>
-      </c>
-      <c r="F54" t="inlineStr">
-        <is>
-          <t>MCQ</t>
-        </is>
-      </c>
-      <c r="G54" t="inlineStr">
-        <is>
-          <t>Fe (II) chloride and hydrogen gas</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>SU0JKR</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>A reaction of hyrdogen with water to form water is</t>
-        </is>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>Chemistry</t>
-        </is>
-      </c>
-      <c r="D55" t="n">
-        <v>2</v>
-      </c>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>Endothermic reaction, Exothermic reaction, Decomposition reaction, Reaction not feasible</t>
-        </is>
-      </c>
-      <c r="F55" t="inlineStr">
-        <is>
-          <t>MCQ</t>
-        </is>
-      </c>
-      <c r="G55" t="inlineStr">
-        <is>
-          <t>Exothermic reaction</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>52CCC0</t>
-        </is>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>What is observed when a solution of potassium Iodide is added to silver nitrate solution ?</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>Chemistry</t>
-        </is>
-      </c>
-      <c r="D56" t="n">
-        <v>2</v>
-      </c>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t>No reaction takes place, White precipitate of silver iodide is formed, yellow precipitate of Agl is formed, Agl is soluble in water</t>
-        </is>
-      </c>
-      <c r="F56" t="inlineStr">
-        <is>
-          <t>MCQ</t>
-        </is>
-      </c>
-      <c r="G56" t="inlineStr">
-        <is>
-          <t>yellow precipitate of Agl is formed</t>
-        </is>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>FCYNBD</t>
-        </is>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>Give the ratio in which hydrogen and oxygen are present in water by volume.</t>
-        </is>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>Chemistry</t>
-        </is>
-      </c>
-      <c r="D57" t="n">
-        <v>2</v>
-      </c>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>1:2, 1:1, 2:1, 1:8</t>
-        </is>
-      </c>
-      <c r="F57" t="inlineStr">
-        <is>
-          <t>MCQ</t>
-        </is>
-      </c>
-      <c r="G57" t="inlineStr">
-        <is>
-          <t>2:1</t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>1MFZCL</t>
-        </is>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>To facilitate the electrolysis of water we add a few drops of acids like sulfuric acid or salts like NaCl because :</t>
-        </is>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>Chemistry</t>
-        </is>
-      </c>
-      <c r="D58" t="n">
-        <v>2</v>
-      </c>
-      <c r="E58" t="inlineStr">
-        <is>
-          <t>It acts as a catalyst, It prevents the decomposition of electrodes used, It increase the electrical conductivity of water, None</t>
-        </is>
-      </c>
-      <c r="F58" t="inlineStr">
-        <is>
-          <t>MCQ</t>
-        </is>
-      </c>
-      <c r="G58" t="inlineStr">
-        <is>
-          <t>It increase the electrical conductivity of water</t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>GIVDY0</t>
-        </is>
-      </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>Which of the following is a displacement reaction ?</t>
-        </is>
-      </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>Chemistry</t>
-        </is>
-      </c>
-      <c r="D59" t="n">
-        <v>2</v>
-      </c>
-      <c r="E59" t="inlineStr">
-        <is>
-          <t>Zn + CuSO4 -&gt; ZnSo4, BaCl2 (aq) + Na2SO4 (aq) -&gt; BaSO4 (s) +  2Nacl(aq), H2 + O2 -&gt; H2O, Zn + CuSO4 -&gt; ZnSO4 + Cu</t>
-        </is>
-      </c>
-      <c r="F59" t="inlineStr">
-        <is>
-          <t>MCQ</t>
-        </is>
-      </c>
-      <c r="G59" t="inlineStr">
-        <is>
-          <t>Zn + CuSO4 -&gt; ZnSO4 + Cu</t>
-        </is>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>Y8MT2F</t>
-        </is>
-      </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>Which one is not type of decomposition reaction ?</t>
-        </is>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>Chemistry</t>
-        </is>
-      </c>
-      <c r="D60" t="n">
-        <v>2</v>
-      </c>
-      <c r="E60" t="inlineStr">
-        <is>
-          <t>Heat, Electricity, Light, Water</t>
-        </is>
-      </c>
-      <c r="F60" t="inlineStr">
-        <is>
-          <t>MCQ</t>
-        </is>
-      </c>
-      <c r="G60" t="inlineStr">
-        <is>
-          <t>Water</t>
-        </is>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>EYRTUS</t>
-        </is>
-      </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>Complete the following decomposition reaction
-2FeSO4 --&gt; Fe2O3 + X + Y</t>
-        </is>
-      </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>Chemistry</t>
-        </is>
-      </c>
-      <c r="D61" t="n">
-        <v>2</v>
-      </c>
-      <c r="E61" t="inlineStr">
-        <is>
-          <t>CO2, CO3, NO2, NO3, H2O, H2, SO2, SO3</t>
-        </is>
-      </c>
-      <c r="F61" t="inlineStr">
-        <is>
-          <t>MCQ</t>
-        </is>
-      </c>
-      <c r="G61" t="inlineStr">
-        <is>
-          <t>SO2, SO3</t>
-        </is>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>C2GF8K</t>
-        </is>
-      </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>Which reaction is not a characteristic of a chemical change</t>
-        </is>
-      </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>Chemistry</t>
-        </is>
-      </c>
-      <c r="D62" t="n">
-        <v>2</v>
-      </c>
-      <c r="E62" t="inlineStr">
-        <is>
-          <t>Mg + O2 -&gt; MgO2, Au + H2O -&gt; Au(OH)2, C + O2 -&gt; CO2, None of above</t>
-        </is>
-      </c>
-      <c r="F62" t="inlineStr">
-        <is>
-          <t>MCQ</t>
-        </is>
-      </c>
-      <c r="G62" t="inlineStr">
-        <is>
-          <t>Au + H2O -&gt; Au(OH)2</t>
-        </is>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>DSN9EP</t>
-        </is>
-      </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>Which is not a type of chemical reaction</t>
-        </is>
-      </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>Chemistry</t>
-        </is>
-      </c>
-      <c r="D63" t="n">
-        <v>2</v>
-      </c>
-      <c r="E63" t="inlineStr">
-        <is>
-          <t>combination, displacement, decompositon, None of Above</t>
-        </is>
-      </c>
-      <c r="F63" t="inlineStr">
-        <is>
-          <t>MCQ</t>
-        </is>
-      </c>
-      <c r="G63" t="inlineStr">
-        <is>
-          <t>None of Above</t>
-        </is>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>2B8N2Y</t>
-        </is>
-      </c>
-      <c r="B64" t="inlineStr">
-        <is>
-          <t>Burning of Coal is</t>
-        </is>
-      </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>Chemistry</t>
-        </is>
-      </c>
-      <c r="D64" t="n">
-        <v>2</v>
-      </c>
-      <c r="E64" t="inlineStr">
-        <is>
-          <t>Displacement, Decomposition, Combination, All of Above</t>
-        </is>
-      </c>
-      <c r="F64" t="inlineStr">
-        <is>
-          <t>MCQ</t>
-        </is>
-      </c>
-      <c r="G64" t="inlineStr">
-        <is>
-          <t>Combination</t>
-        </is>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>4ZSZ26</t>
-        </is>
-      </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>An example of exothermic reaction is</t>
-        </is>
-      </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>Chemistry</t>
-        </is>
-      </c>
-      <c r="D65" t="n">
-        <v>2</v>
-      </c>
-      <c r="E65" t="inlineStr">
-        <is>
-          <t>CaO + H2O -&gt; Ca(OH)2, 2Mg + O2 -&gt; 2MgO, 4Fe + 3O2 -&gt; 2Fe2O3, None</t>
-        </is>
-      </c>
-      <c r="F65" t="inlineStr">
-        <is>
-          <t>MCQ</t>
-        </is>
-      </c>
-      <c r="G65" t="inlineStr">
-        <is>
-          <t>CaO + H2O -&gt; Ca(OH)2</t>
-        </is>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="inlineStr">
-        <is>
-          <t>ZC2KSD</t>
-        </is>
-      </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>Symbol A used while representing some chemical changes stands for</t>
-        </is>
-      </c>
-      <c r="C66" t="inlineStr">
-        <is>
-          <t>Chemistry</t>
-        </is>
-      </c>
-      <c r="D66" t="n">
-        <v>2</v>
-      </c>
-      <c r="E66" t="inlineStr">
-        <is>
-          <t>Light, Heat, Catalysts, Pressure</t>
-        </is>
-      </c>
-      <c r="F66" t="inlineStr">
-        <is>
-          <t>MCQ</t>
-        </is>
-      </c>
-      <c r="G66" t="inlineStr">
-        <is>
-          <t>Heat</t>
-        </is>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>DJSM28</t>
-        </is>
-      </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>Which of the following statements is/are correct ?</t>
-        </is>
-      </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>Chemistry</t>
-        </is>
-      </c>
-      <c r="D67" t="n">
-        <v>2</v>
-      </c>
-      <c r="E67" t="inlineStr">
-        <is>
-          <t>A chemical equation tells us about the substances involved in a reaction, A chemical equation informs us about the symbols and formulae of the substances involved in a reaction, A chemical equation tells about the atoms or molecules of the reactants and products in a reaction, All of Above</t>
-        </is>
-      </c>
-      <c r="F67" t="inlineStr">
-        <is>
-          <t>MCQ</t>
-        </is>
-      </c>
-      <c r="G67" t="inlineStr">
-        <is>
-          <t>All of Above</t>
-        </is>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>40VAVV</t>
-        </is>
-      </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>Which of the following is a combustion reaction</t>
-        </is>
-      </c>
-      <c r="C68" t="inlineStr">
-        <is>
-          <t>Chemistry</t>
-        </is>
-      </c>
-      <c r="D68" t="n">
-        <v>2</v>
-      </c>
-      <c r="E68" t="inlineStr">
-        <is>
-          <t>Burning of Petrol, Boiling of water, Melting of wax, None of these</t>
-        </is>
-      </c>
-      <c r="F68" t="inlineStr">
-        <is>
-          <t>MCQ</t>
-        </is>
-      </c>
-      <c r="G68" t="inlineStr">
-        <is>
-          <t>Burning of Petrol</t>
-        </is>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>9E8OMG</t>
-        </is>
-      </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>Neutralization reaction is an example of</t>
-        </is>
-      </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t>Chemistry</t>
-        </is>
-      </c>
-      <c r="D69" t="n">
-        <v>2</v>
-      </c>
-      <c r="E69" t="inlineStr">
-        <is>
-          <t>exothermic reaction, endothermic reaction, oxidation, None of these</t>
-        </is>
-      </c>
-      <c r="F69" t="inlineStr">
-        <is>
-          <t>MCQ</t>
-        </is>
-      </c>
-      <c r="G69" t="inlineStr">
-        <is>
-          <t>exothermic reaction</t>
-        </is>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>RH8J7P</t>
-        </is>
-      </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>Which of the following reactions involves the combination of two elements ?</t>
-        </is>
-      </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t>Chemistry</t>
-        </is>
-      </c>
-      <c r="D70" t="n">
-        <v>2</v>
-      </c>
-      <c r="E70" t="inlineStr">
-        <is>
-          <t>CaCo3 + Co2 -&gt; CaCo3, 4Na + O2 -&gt; 2Na2O, SO2 + 1/2O2 -&gt; SO3, NH3 + HCL -&gt; NH4Cl</t>
-        </is>
-      </c>
-      <c r="F70" t="inlineStr">
-        <is>
-          <t>MCQ</t>
-        </is>
-      </c>
-      <c r="G70" t="inlineStr">
-        <is>
-          <t>4Na + O2 -&gt; 2Na2O</t>
+          <t>government</t>
         </is>
       </c>
     </row>

</xml_diff>